<commit_message>
update insert all function for new template
still working on it. not finished yet
</commit_message>
<xml_diff>
--- a/Unit_Budget/Python_File/New Template v0.2.xlsx
+++ b/Unit_Budget/Python_File/New Template v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Downloads\UWA\2021-s2\Professional Computing CITS5206\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1398C467-786F-49C4-BC73-E2E0611B97A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C5CF59-1FDF-43DF-BE97-AE3F47CCE802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
   <si>
     <t>Unit details</t>
   </si>
@@ -290,6 +290,10 @@
   </si>
   <si>
     <t>HOURS PER ACTIVITY</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -304,7 +308,7 @@
     <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="178" formatCode="[$$-C09]#,##0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +376,15 @@
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -516,7 +529,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
@@ -548,7 +561,6 @@
     </xf>
     <xf numFmtId="176" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -585,6 +597,8 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -4178,8 +4192,8 @@
   </sheetPr>
   <dimension ref="A3:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4214,35 +4228,35 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="38">
         <f>B11</f>
         <v>2021</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="38">
         <f>B11-1</f>
         <v>2020</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="37" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="37" t="s">
         <v>10</v>
       </c>
       <c r="D8">
         <v>410</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="37" t="s">
         <v>11</v>
       </c>
       <c r="F8">
@@ -4250,76 +4264,81 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="str">
         <f>IFERROR(VLOOKUP(B7,'[1]Budget 2019'!C:E,3,FALSE)," ")</f>
         <v>Software Engineering with Java</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C9" s="37"/>
+      <c r="E9" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="37" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="3">
         <v>65325</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="37" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="3">
         <v>50050</v>
       </c>
-      <c r="Q10" s="35"/>
+      <c r="Q10" s="34"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="37" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>2021</v>
       </c>
-      <c r="E11" t="s">
+      <c r="C11" s="37"/>
+      <c r="E11" s="37" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
       </c>
-      <c r="Q11" s="35"/>
+      <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="37" t="s">
         <v>69</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="Q12" s="35"/>
+      <c r="Q12" s="34"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q13" s="35"/>
+      <c r="A13" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q13" s="34"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q14" s="35"/>
+      <c r="Q14" s="34"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q15" s="35"/>
+      <c r="Q15" s="34"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q16" s="35"/>
+      <c r="Q16" s="34"/>
     </row>
     <row r="17" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>61</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -4345,7 +4364,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="26" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -4371,7 +4390,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>73</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -4397,7 +4416,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>74</v>
       </c>
       <c r="B20" s="8">
@@ -4423,10 +4442,10 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="31"/>
+      <c r="B25" s="30"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -4435,7 +4454,7 @@
       <c r="B26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="20" t="s">
         <v>63</v>
       </c>
       <c r="D26" s="6" t="s">
@@ -4459,12 +4478,12 @@
       <c r="J26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="33" t="s">
+      <c r="K26" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="25" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="7">
@@ -4474,7 +4493,9 @@
         <f>12*B27</f>
         <v>48</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="7">
+        <v>48</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -4486,7 +4507,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="26" t="s">
         <v>32</v>
       </c>
       <c r="B28" s="7">
@@ -4497,15 +4518,23 @@
         <v>24</v>
       </c>
       <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="8"/>
+      <c r="E28" s="8">
+        <v>4</v>
+      </c>
+      <c r="F28" s="8">
+        <v>8</v>
+      </c>
+      <c r="G28" s="7">
+        <v>4</v>
+      </c>
+      <c r="H28" s="8">
+        <v>8</v>
+      </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="7">
@@ -4517,14 +4546,22 @@
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
+      <c r="F29" s="8">
+        <v>4</v>
+      </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="H29" s="8">
+        <v>4</v>
+      </c>
+      <c r="I29" s="8">
+        <v>8</v>
+      </c>
+      <c r="J29" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>60</v>
       </c>
       <c r="B30" s="7">
@@ -4535,15 +4572,23 @@
         <v>72</v>
       </c>
       <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8">
+        <v>12</v>
+      </c>
       <c r="F30" s="8"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
+      <c r="G30" s="7">
+        <v>36</v>
+      </c>
+      <c r="H30" s="8">
+        <v>12</v>
+      </c>
+      <c r="I30" s="8">
+        <v>12</v>
+      </c>
       <c r="J30" s="8"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="26" t="s">
         <v>59</v>
       </c>
       <c r="B31" s="7">
@@ -4554,18 +4599,30 @@
         <v>246</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="E31" s="8">
+        <v>41</v>
+      </c>
+      <c r="F31" s="8">
+        <v>41</v>
+      </c>
+      <c r="G31" s="7">
+        <v>41</v>
+      </c>
+      <c r="H31" s="8">
+        <v>41</v>
+      </c>
+      <c r="I31" s="8">
+        <v>41</v>
+      </c>
+      <c r="J31" s="8">
+        <v>41</v>
+      </c>
       <c r="K31" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>34</v>
       </c>
       <c r="B32" s="7">
@@ -4576,15 +4633,21 @@
         <v>24</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
+      <c r="E32" s="8">
+        <v>12</v>
+      </c>
+      <c r="F32" s="8">
+        <v>6</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
+      <c r="I32" s="8">
+        <v>6</v>
+      </c>
       <c r="J32" s="8"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>66</v>
       </c>
       <c r="B33" s="7">
@@ -4596,9 +4659,15 @@
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
+      <c r="F33" s="8">
+        <v>6</v>
+      </c>
+      <c r="G33" s="7">
+        <v>12</v>
+      </c>
+      <c r="H33" s="8">
+        <v>6</v>
+      </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="P33" t="s">
@@ -4606,7 +4675,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="26" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="7">
@@ -4617,8 +4686,12 @@
         <v>8</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
+      <c r="E34" s="8">
+        <v>4</v>
+      </c>
+      <c r="F34" s="8">
+        <v>4</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -4628,7 +4701,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="26" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="7">
@@ -4639,15 +4712,19 @@
         <v>12</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="E35" s="8">
+        <v>6</v>
+      </c>
+      <c r="F35" s="8">
+        <v>6</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="7">
@@ -4657,7 +4734,9 @@
         <f>B36</f>
         <v>3</v>
       </c>
-      <c r="D36" s="8"/>
+      <c r="D36" s="8">
+        <v>3</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="7"/>
@@ -4669,7 +4748,7 @@
       </c>
     </row>
     <row r="37" spans="1:16" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="7">
@@ -4679,7 +4758,9 @@
         <f t="shared" ref="C37:C39" si="1">B37</f>
         <v>10</v>
       </c>
-      <c r="D37" s="8"/>
+      <c r="D37" s="8">
+        <v>10</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37" s="7"/>
@@ -4688,7 +4769,7 @@
       <c r="J37" s="8"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="7">
@@ -4698,7 +4779,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="D38" s="8"/>
+      <c r="D38" s="8">
+        <v>10</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
       <c r="G38" s="7"/>
@@ -4707,7 +4790,7 @@
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="7">
@@ -4717,7 +4800,9 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D39" s="8"/>
+      <c r="D39" s="8">
+        <v>20</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="7"/>
@@ -4726,41 +4811,41 @@
       <c r="J39" s="8"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25">
+      <c r="B40" s="24"/>
+      <c r="C40" s="24">
         <f>SUM(C27:C39)</f>
         <v>525</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
     </row>
     <row r="44" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="31"/>
+      <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -4769,7 +4854,7 @@
       <c r="B45" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="20" t="s">
         <v>53</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -4793,18 +4878,18 @@
       <c r="J45" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K45" s="33" t="s">
+      <c r="K45" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="23">
+      <c r="B46" s="22">
         <v>0.25</v>
       </c>
-      <c r="C46" s="22">
+      <c r="C46" s="21">
         <f>B46*D8</f>
         <v>102.5</v>
       </c>
@@ -4833,10 +4918,10 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="25.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="23">
+      <c r="B47" s="22">
         <v>0.25</v>
       </c>
       <c r="C47">
@@ -4868,10 +4953,10 @@
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="23">
+      <c r="B48" s="22">
         <v>0.5</v>
       </c>
       <c r="C48">
@@ -4903,68 +4988,68 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25">
+      <c r="B49" s="24"/>
+      <c r="C49" s="24">
         <f>SUM(C46:C48)</f>
         <v>410</v>
       </c>
-      <c r="D49" s="34">
+      <c r="D49" s="33">
         <f t="shared" ref="D49:J49" si="3">SUM(D46:D48)</f>
         <v>30</v>
       </c>
-      <c r="E49" s="34">
+      <c r="E49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
-      <c r="F49" s="34">
+      <c r="F49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
-      <c r="H49" s="34">
+      <c r="H49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
-      <c r="I49" s="34">
+      <c r="I49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
-      <c r="J49" s="34">
+      <c r="J49" s="33">
         <f t="shared" si="3"/>
         <v>63.333333333333336</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
+    <row r="50" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="36">
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="35">
         <f>D49*Q11</f>
         <v>0</v>
       </c>
-      <c r="E50" s="37">
+      <c r="E50" s="36">
         <f>E49*Q12</f>
         <v>0</v>
       </c>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24"/>
       <c r="K50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30"/>
+    <row r="51" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="29"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
@@ -4980,17 +5065,17 @@
       <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
     </row>
     <row r="54" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="32" t="s">
+      <c r="A54" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="31"/>
+      <c r="B54" s="30"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
@@ -5013,13 +5098,15 @@
       <c r="A56" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="2"/>
+      <c r="B56" s="2">
+        <v>20</v>
+      </c>
       <c r="C56" s="11">
         <v>75</v>
       </c>
       <c r="D56" s="12">
         <f>B56*C56</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="E56" s="13"/>
     </row>
@@ -5027,17 +5114,19 @@
       <c r="A57" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>10</v>
+      </c>
       <c r="C57" s="11">
         <v>50</v>
       </c>
       <c r="D57" s="12">
         <f>B57*C57</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E57" s="13"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
@@ -5051,8 +5140,8 @@
       <c r="E58" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J58" s="19"/>
-      <c r="K58" s="20"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="19"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
@@ -5076,22 +5165,22 @@
       <c r="E61" s="9"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="A63" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="24"/>
+      <c r="E63" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Complete Insert All function
the insert all function now working with new template. In addition, fix the problem of duplicate insert, if user try to insert the same excel file more than once
</commit_message>
<xml_diff>
--- a/Unit_Budget/Python_File/New Template v0.2.xlsx
+++ b/Unit_Budget/Python_File/New Template v0.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Downloads\UWA\2021-s2\Professional Computing CITS5206\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\Unit_Budget_Planner\Unit_Budget\Python_File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCE2F48-0D6C-4271-AA90-BB63721C5474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DEAB7-6E7B-4D96-8F0C-D752176723BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>Unit details</t>
   </si>
@@ -196,10 +196,6 @@
     <t>Copied from 2020 budget</t>
   </si>
   <si>
-    <t>Note: for Non-salary cost. The insert function will look up to 6 costs for now.</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Total Cost</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -290,11 +286,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Comment</t>
+    <t>Number of Teaching Staff</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Number of Teaching Staff</t>
+    <t>Number of NonSalaryCost</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -4192,7 +4188,7 @@
   <dimension ref="A3:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4314,7 +4310,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -4324,6 +4320,9 @@
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>76</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
       </c>
       <c r="Q13" s="34"/>
     </row>
@@ -4338,10 +4337,10 @@
     </row>
     <row r="17" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>19</v>
@@ -4364,7 +4363,7 @@
     </row>
     <row r="18" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>18</v>
@@ -4390,10 +4389,10 @@
     </row>
     <row r="19" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>21</v>
@@ -4416,7 +4415,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="8">
         <v>0</v>
@@ -4442,19 +4441,19 @@
     </row>
     <row r="25" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="30"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>17</v>
@@ -4478,7 +4477,7 @@
         <v>27</v>
       </c>
       <c r="K26" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -4502,7 +4501,7 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -4561,7 +4560,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="7">
         <v>1</v>
@@ -4588,7 +4587,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="7">
         <v>2</v>
@@ -4617,7 +4616,7 @@
         <v>41</v>
       </c>
       <c r="K31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -4647,7 +4646,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
@@ -4670,7 +4669,7 @@
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="P33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -4696,7 +4695,7 @@
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -4743,12 +4742,12 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="7">
         <v>10</v>
@@ -4769,7 +4768,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" s="7">
         <v>10</v>
@@ -4790,7 +4789,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B39" s="7">
         <v>20</v>
@@ -4828,7 +4827,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
@@ -4842,19 +4841,19 @@
     </row>
     <row r="44" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="20" t="s">
         <v>52</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>17</v>
@@ -4878,7 +4877,7 @@
         <v>27</v>
       </c>
       <c r="K45" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -5026,7 +5025,7 @@
     </row>
     <row r="50" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
@@ -5044,7 +5043,7 @@
       <c r="I50" s="24"/>
       <c r="J50" s="24"/>
       <c r="K50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -5061,9 +5060,6 @@
       <c r="K51"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>47</v>
-      </c>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -5072,7 +5068,7 @@
     </row>
     <row r="54" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="30"/>
     </row>
@@ -5174,7 +5170,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B63" s="24"/>
       <c r="C63" s="24"/>

</xml_diff>

<commit_message>
disable the button that still working on progress
</commit_message>
<xml_diff>
--- a/Unit_Budget/Python_File/New Template v0.2.xlsx
+++ b/Unit_Budget/Python_File/New Template v0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\Unit_Budget_Planner\Unit_Budget\Python_File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameam/Desktop/OneDrive/Desktop/Professional/project1/Unit_Budget_Planner/Unit_Budget/Python_File/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DEAB7-6E7B-4D96-8F0C-D752176723BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC4425-8AFE-2C4D-839B-9E47E417EA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28600" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.2" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -301,22 +303,22 @@
   <numFmts count="5">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="[$$-C09]#,##0;[Red][$$-C09]#,##0"/>
-    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="178" formatCode="[$$-C09]#,##0"/>
+    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0;[Red][$$-C09]#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="[$$-C09]#,##0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -325,7 +327,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -334,13 +336,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -348,7 +350,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -356,14 +358,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -371,7 +373,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -379,7 +381,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -530,7 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -548,15 +550,15 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4187,42 +4189,42 @@
   </sheetPr>
   <dimension ref="A3:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.21875" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" customWidth="1"/>
+    <col min="18" max="18" width="8.83203125" customWidth="1"/>
     <col min="19" max="19" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
         <v>1</v>
       </c>
@@ -4238,7 +4240,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>3</v>
       </c>
@@ -4258,7 +4260,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>5</v>
       </c>
@@ -4271,7 +4273,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>6</v>
       </c>
@@ -4292,7 +4294,7 @@
       </c>
       <c r="Q10" s="34"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>8</v>
       </c>
@@ -4308,7 +4310,7 @@
       </c>
       <c r="Q11" s="34"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>75</v>
       </c>
@@ -4317,7 +4319,7 @@
       </c>
       <c r="Q12" s="34"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="37" t="s">
         <v>76</v>
       </c>
@@ -4326,16 +4328,16 @@
       </c>
       <c r="Q13" s="34"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q14" s="34"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q15" s="34"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="Q16" s="34"/>
     </row>
-    <row r="17" spans="1:11" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>60</v>
       </c>
@@ -4361,7 +4363,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
         <v>70</v>
       </c>
@@ -4387,7 +4389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
         <v>71</v>
       </c>
@@ -4413,7 +4415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
         <v>72</v>
       </c>
@@ -4439,13 +4441,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B25" s="30"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>61</v>
       </c>
@@ -4480,7 +4482,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>4</v>
       </c>
@@ -4504,7 +4506,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
         <v>32</v>
       </c>
@@ -4531,7 +4533,7 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="26" t="s">
         <v>33</v>
       </c>
@@ -4558,7 +4560,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
         <v>59</v>
       </c>
@@ -4585,7 +4587,7 @@
       </c>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="26" t="s">
         <v>58</v>
       </c>
@@ -4619,7 +4621,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
         <v>34</v>
       </c>
@@ -4644,7 +4646,7 @@
       </c>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="26" t="s">
         <v>65</v>
       </c>
@@ -4672,7 +4674,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="26" t="s">
         <v>35</v>
       </c>
@@ -4698,7 +4700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="26" t="s">
         <v>36</v>
       </c>
@@ -4721,7 +4723,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="26" t="s">
         <v>37</v>
       </c>
@@ -4745,7 +4747,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
         <v>53</v>
       </c>
@@ -4766,7 +4768,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
         <v>54</v>
       </c>
@@ -4787,7 +4789,7 @@
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>55</v>
       </c>
@@ -4808,7 +4810,7 @@
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
         <v>16</v>
       </c>
@@ -4825,7 +4827,7 @@
       <c r="I40" s="24"/>
       <c r="J40" s="24"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="27" t="s">
         <v>47</v>
       </c>
@@ -4839,13 +4841,13 @@
       <c r="I41" s="24"/>
       <c r="J41" s="24"/>
     </row>
-    <row r="44" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>56</v>
       </c>
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>61</v>
       </c>
@@ -4880,7 +4882,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="28" t="s">
         <v>29</v>
       </c>
@@ -4915,7 +4917,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="25.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="28" t="s">
         <v>30</v>
       </c>
@@ -4950,7 +4952,7 @@
         <v>15.833333333333334</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="28" t="s">
         <v>31</v>
       </c>
@@ -4985,7 +4987,7 @@
         <v>31.666666666666668</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
         <v>16</v>
       </c>
@@ -5023,7 +5025,7 @@
         <v>63.333333333333336</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="18" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="27" t="s">
         <v>47</v>
       </c>
@@ -5046,7 +5048,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="29"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -5059,20 +5061,20 @@
       <c r="J51"/>
       <c r="K51"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
     </row>
-    <row r="54" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B54" s="30"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
         <v>38</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
         <v>43</v>
       </c>
@@ -5105,7 +5107,7 @@
       </c>
       <c r="E56" s="13"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>44</v>
       </c>
@@ -5123,7 +5125,7 @@
       <c r="J57" s="18"/>
       <c r="K57" s="18"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="s">
         <v>45</v>
       </c>
@@ -5138,28 +5140,28 @@
       <c r="J58" s="18"/>
       <c r="K58" s="19"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="23" t="s">
         <v>16</v>
       </c>
@@ -5168,7 +5170,7 @@
       <c r="D62" s="24"/>
       <c r="E62" s="24"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
         <v>47</v>
       </c>

</xml_diff>